<commit_message>
FEAT: Balance tower speed again
</commit_message>
<xml_diff>
--- a/doc/Game Balance.xlsx
+++ b/doc/Game Balance.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\编程\Projects\Sunaba\Defender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Programming\Projects\Sunaba\Defender\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A2079C-2945-4362-B6C4-7AD670FF9A09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE2FC78-8407-4A94-BEB5-2684DE5C0784}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" xr2:uid="{6AD152CE-BB64-4651-A9EB-E7D9A01DA758}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" activeTab="1" xr2:uid="{6AD152CE-BB64-4651-A9EB-E7D9A01DA758}"/>
   </bookViews>
   <sheets>
     <sheet name="Enemy" sheetId="1" r:id="rId1"/>
     <sheet name="Tower" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" concurrentManualCount="2"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Radius</t>
     <phoneticPr fontId="1"/>
@@ -69,10 +70,6 @@
   </si>
   <si>
     <t>Life</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Speed Level Buff</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -127,13 +124,109 @@
     <t>75=5*15</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Equilibrated Shoot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>敵が集まるところに強い砲台を配置</t>
+    <rPh sb="0" eb="1">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アツ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ツヨ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ホウダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ハイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>遠い敵は砲台を取り外して避ける</t>
+    <rPh sb="0" eb="1">
+      <t>トオ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ホウダイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>砲台を自爆から守るために捨て砲台を配置</t>
+    <rPh sb="0" eb="2">
+      <t>ホウダイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジバク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>マモ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホウダイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ハイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>砲台は低レベルのとき強化の恩恵が多いから一つ強力のやつより複数</t>
+    <rPh sb="0" eb="2">
+      <t>ホウダイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>テイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>キョウカ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>オンケイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>キョウリョク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>フクスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -202,7 +295,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -212,13 +305,25 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="176" formatCode="0.0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="0.00_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.0_ "/>
     </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="0.0_ "/>
@@ -425,37 +530,37 @@
             <c:numRef>
               <c:f>Tower!$B$5:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>41.813052890456184</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>27.904554138779094</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22.469541179956238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>19.39277515135554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>17.351997874691335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>15.872155148205277</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>14.73572396181576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>13.827369567036138</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>13.079555501165361</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>12.449781248667259</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,7 +666,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -599,6 +704,460 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1085955976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>Shoot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP" baseline="0"/>
+              <a:t> Equilibrium</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tower!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.7143575756999034</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.054727044622879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.938101824688552</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.101386805316782</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.818352632086707</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.225530548109404</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.402306745219235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.399510104077422</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.25192851240886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.98456800579995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1BB0-4185-9600-F1FFEE9DABE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>EQ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tower!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tower!$D$5:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0DBD-4B65-9312-BC3117A5DB7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="914080048"/>
+        <c:axId val="914071848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="914080048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="914071848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="914071848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="914080048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -694,6 +1253,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1210,20 +1809,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>36195</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>613410</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>74295</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1287780</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>203835</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1243,6 +2358,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>384810</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>211455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9AA7176-B26B-4A34-966D-86E72FF7004D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1282,30 +2433,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F16D103B-8575-41F0-AE9E-73461599B2C5}" name="テーブル2" displayName="テーブル2" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{109998D9-ADBB-4B6C-87B0-DB392D115668}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F16D103B-8575-41F0-AE9E-73461599B2C5}" name="テーブル2" displayName="テーブル2" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{109998D9-ADBB-4B6C-87B0-DB392D115668}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{23BC00C6-244C-4608-9BA2-C548EA7A78C1}" name="Height"/>
     <tableColumn id="2" xr3:uid="{4EA36D01-4860-41E6-9DFC-D97D3B401540}" name="Base Speed"/>
-    <tableColumn id="4" xr3:uid="{DD3EF97C-B535-48EE-9753-0D0128110FAB}" name="Speed Level Buff"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{16E28406-1DB1-4718-B732-F959E32F6A4F}" name="テーブル3" displayName="テーブル3" ref="A4:D14" totalsRowShown="0">
-  <autoFilter ref="A4:D14" xr:uid="{A1815F41-EAD6-4C06-A656-27A00E6CFACB}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{16E28406-1DB1-4718-B732-F959E32F6A4F}" name="テーブル3" displayName="テーブル3" ref="A4:E14" totalsRowShown="0">
+  <autoFilter ref="A4:E14" xr:uid="{A1815F41-EAD6-4C06-A656-27A00E6CFACB}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6A7F8E12-A05C-4EAF-8982-B1077EC711CB}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{9979FC82-4591-4A02-80C7-1748B74F4DF0}" name="Speed">
-      <calculatedColumnFormula>テーブル2[Base Speed]-テーブル3[[#This Row],[Level]]*テーブル2[Speed Level Buff]</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{9979FC82-4591-4A02-80C7-1748B74F4DF0}" name="Speed" dataDxfId="1">
+      <calculatedColumnFormula>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{60D3B640-777A-409A-B9F7-8B66EC69AF77}" name="Bullets Shoot till Enemy Arrival" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{60D3B640-777A-409A-B9F7-8B66EC69AF77}" name="Bullets Shoot till Enemy Arrival" dataDxfId="3">
       <calculatedColumnFormula>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" xr3:uid="{29096A4E-D9F4-48B3-8DCD-FB0457D0D19B}" name="Equilibrated Shoot" dataDxfId="2">
+      <calculatedColumnFormula>テーブル3[Level]*5</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{92538962-7F1E-4D4C-B21E-A38B37AAE60B}" name="Expected Shoot" dataDxfId="0">
-      <calculatedColumnFormula>テーブル3[[#This Row],[Level]]*5*1.2</calculatedColumnFormula>
+      <calculatedColumnFormula>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1611,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54724089-3523-48E2-9C89-EB95F1721D91}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1667,13 +2820,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.85">
@@ -1681,7 +2834,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.85">
@@ -1689,7 +2842,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.85">
@@ -1697,7 +2850,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.85">
@@ -1705,7 +2858,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.85">
@@ -1713,7 +2866,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.85">
@@ -1721,14 +2874,14 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <f>(350-15)/25</f>
         <v>13.4</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.85">
@@ -1740,7 +2893,7 @@
         <v>80.400000000000006</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.85">
@@ -1748,7 +2901,7 @@
         <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.85">
@@ -1756,7 +2909,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.85">
@@ -1777,10 +2930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D376B921-6970-4F1C-9BC5-6A0A32D91462}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
@@ -1788,32 +2941,27 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.37890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" ht="18.3" x14ac:dyDescent="0.85">
+    <row r="4" spans="1:5" ht="18.3" x14ac:dyDescent="0.85">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1823,171 +2971,224 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>45</v>
+      <c r="B5" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>41.813052890456184</v>
       </c>
       <c r="C5" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>7.9555555555555557</v>
-      </c>
-      <c r="D5">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>6</v>
+        <v>8.7143575756999052</v>
+      </c>
+      <c r="D5" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>8.7143575756999034</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>30</v>
+      <c r="B6" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>27.904554138779094</v>
       </c>
       <c r="C6" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>12.933333333333334</v>
-      </c>
-      <c r="D6">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>12</v>
+        <v>14.054727044622879</v>
+      </c>
+      <c r="D6" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>14.054727044622879</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>21</v>
+      <c r="B7" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>22.469541179956238</v>
       </c>
       <c r="C7" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>19.333333333333332</v>
-      </c>
-      <c r="D7">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>18</v>
+        <v>17.938101824688552</v>
+      </c>
+      <c r="D7" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>17.938101824688552</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>17</v>
+      <c r="B8" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>19.39277515135554</v>
       </c>
       <c r="C8" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>24.352941176470587</v>
-      </c>
-      <c r="D8">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>24</v>
+        <v>21.101386805316782</v>
+      </c>
+      <c r="D8" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>21.101386805316782</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>14</v>
+      <c r="B9" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>17.351997874691335</v>
       </c>
       <c r="C9" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>30</v>
+        <v>23.818352632086707</v>
+      </c>
+      <c r="D9" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>25</v>
+      </c>
+      <c r="E9" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>23.818352632086707</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10">
-        <v>11</v>
+      <c r="B10" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>15.872155148205277</v>
       </c>
       <c r="C10" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>38.727272727272727</v>
-      </c>
-      <c r="D10">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>36</v>
+        <v>26.225530548109404</v>
+      </c>
+      <c r="D10" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>30</v>
+      </c>
+      <c r="E10" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>26.225530548109404</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>10</v>
+      <c r="B11" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>14.73572396181576</v>
       </c>
       <c r="C11" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>42.8</v>
-      </c>
-      <c r="D11">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>42</v>
+        <v>28.402306745219235</v>
+      </c>
+      <c r="D11" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>35</v>
+      </c>
+      <c r="E11" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>28.402306745219235</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>9</v>
+      <c r="B12" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>13.827369567036138</v>
       </c>
       <c r="C12" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>47.777777777777779</v>
-      </c>
-      <c r="D12">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>48</v>
+        <v>30.399510104077422</v>
+      </c>
+      <c r="D12" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>40</v>
+      </c>
+      <c r="E12" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>30.399510104077422</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13">
-        <v>8</v>
+      <c r="B13" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>13.079555501165361</v>
       </c>
       <c r="C13" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>54</v>
-      </c>
-      <c r="D13">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>54</v>
+        <v>32.25192851240886</v>
+      </c>
+      <c r="D13" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>45</v>
+      </c>
+      <c r="E13" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>32.25192851240886</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14">
-        <v>7</v>
+      <c r="B14" s="4">
+        <f>テーブル1[Time to Collide with Tower]/(テーブル3[[#This Row],[Expected Shoot]] + 2)</f>
+        <v>12.449781248667259</v>
       </c>
       <c r="C14" s="2">
         <f>テーブル1[Time to Collide with Tower]/テーブル3[Speed] - 2</f>
-        <v>62</v>
-      </c>
-      <c r="D14">
-        <f>テーブル3[[#This Row],[Level]]*5*1.2</f>
-        <v>60</v>
+        <v>33.98456800579995</v>
+      </c>
+      <c r="D14" s="2">
+        <f>テーブル3[Level]*5</f>
+        <v>50</v>
+      </c>
+      <c r="E14" s="2">
+        <f>1.1 * POWER(900 * テーブル3[[#This Row],[Level]], 0.4) - 8</f>
+        <v>33.98456800579995</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.85">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A16">
         <f>7*9</f>
         <v>63</v>
@@ -2003,4 +3204,40 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305A29FC-F91A-4B38-AFFC-EF0161C27771}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>